<commit_message>
Atualização dos artefatos para AC 4
</commit_message>
<xml_diff>
--- a/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/17. Análise dos Eventos para cada Cenário.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Mylren\Documents\GitHub\Eng-Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C026878-E031-4E39-AF08-C897AD95123F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC54DAF-6AC6-4988-B718-8C26DDEAF878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A55B0A7-CAD9-48C3-AB1E-DE54A387BEEE}"/>
   </bookViews>
@@ -93,9 +93,6 @@
     <t>Atendente calcula o orçamento e entrega ao Cliente</t>
   </si>
   <si>
-    <t>Atendente gera o boleto do pedido</t>
-  </si>
-  <si>
     <t>Atendente recusa o pedido por falta de estoque</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>x(17)</t>
+  </si>
+  <si>
+    <t>Atendente recebe a resposta do Cliente</t>
   </si>
 </sst>
 </file>
@@ -537,52 +537,61 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -592,9 +601,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -606,22 +612,16 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -941,7 +941,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,22 +957,22 @@
       <c r="B1" s="3"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="16" t="s">
         <v>3</v>
       </c>
@@ -999,10 +999,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="30" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="9">
@@ -1021,8 +1021,8 @@
       <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="9">
         <v>2</v>
       </c>
@@ -1039,33 +1039,33 @@
       <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="23"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="9">
         <v>3</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="17"/>
       <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="19">
         <v>4</v>
       </c>
-      <c r="D6" s="33" t="s">
-        <v>23</v>
+      <c r="D6" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
@@ -1077,18 +1077,18 @@
       <c r="J6" s="18"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="19">
         <v>5</v>
       </c>
-      <c r="D7" s="33" t="s">
-        <v>24</v>
+      <c r="D7" s="22" t="s">
+        <v>23</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="4"/>
@@ -1097,17 +1097,17 @@
       <c r="J7" s="18"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="24" t="s">
+      <c r="A8" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="38" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="20">
         <v>6</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>15</v>
@@ -1119,13 +1119,13 @@
       <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="34"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="20">
         <v>7</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -1137,36 +1137,36 @@
       <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="36" t="s">
+      <c r="A10" s="41"/>
+      <c r="B10" s="46" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="20">
         <v>8</v>
       </c>
-      <c r="D10" s="35" t="s">
-        <v>30</v>
+      <c r="D10" s="23" t="s">
+        <v>29</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
       <c r="G10" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="17"/>
       <c r="J10" s="18"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="25"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="47"/>
       <c r="C11" s="20">
         <v>9</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="4"/>
@@ -1175,35 +1175,35 @@
       <c r="J11" s="18"/>
     </row>
     <row r="12" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="48" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="19">
         <v>10</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="17"/>
       <c r="J12" s="18"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
-      <c r="B13" s="22"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="19">
         <v>11</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>17</v>
@@ -1215,13 +1215,13 @@
       <c r="J13" s="18"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
-      <c r="B14" s="40"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="19">
         <v>12</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="13"/>
@@ -1233,37 +1233,37 @@
       <c r="J14" s="18"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
-      <c r="B15" s="28" t="s">
+      <c r="A15" s="45"/>
+      <c r="B15" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="19">
         <v>13</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="13"/>
       <c r="G15" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="17"/>
       <c r="J15" s="18"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="44" t="s">
+      <c r="A16" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="27" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="20">
         <v>14</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="13" t="s">
@@ -1275,70 +1275,70 @@
       <c r="J16" s="18"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="45"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="20">
         <v>15</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="17"/>
       <c r="J17" s="18"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
-      <c r="B18" s="45"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="20">
         <v>16</v>
       </c>
-      <c r="D18" s="35" t="s">
-        <v>39</v>
+      <c r="D18" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="17"/>
       <c r="J18" s="18"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="48"/>
-      <c r="B19" s="45"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="20">
         <v>17</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="17"/>
       <c r="J19" s="18"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="46"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="20">
         <v>18</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="4"/>
@@ -1348,11 +1348,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="B8:B9"/>
@@ -1360,6 +1355,11 @@
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>